<commit_message>
working login through google, redirect homepage, profile page edit
</commit_message>
<xml_diff>
--- a/TodoList.xlsx
+++ b/TodoList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>register chapter into database</t>
   </si>
@@ -30,9 +30,6 @@
     <t>TODO</t>
   </si>
   <si>
-    <t>send automatic email to members with verification code</t>
-  </si>
-  <si>
     <t>import univerisities &amp; chapters into database</t>
   </si>
   <si>
@@ -42,12 +39,6 @@
     <t>import chapter information fromuploaded  template</t>
   </si>
   <si>
-    <t>have usersverfiy code</t>
-  </si>
-  <si>
-    <t>have users create password</t>
-  </si>
-  <si>
     <t>Roster</t>
   </si>
   <si>
@@ -100,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">logout </t>
-  </si>
-  <si>
-    <t>forgot your password?</t>
   </si>
   <si>
     <t>Chapter Events</t>
@@ -226,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +266,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -281,6 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -632,15 +627,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
     <col min="2" max="2" width="48.6640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
@@ -654,183 +649,169 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1"/>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="90">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" t="s">
-        <v>25</v>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working chap announcements into database, starting food menu, sample profile page
</commit_message>
<xml_diff>
--- a/TodoList.xlsx
+++ b/TodoList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>register chapter into database</t>
   </si>
@@ -144,12 +144,6 @@
     <t>iphone app?</t>
   </si>
   <si>
-    <t>exc add chapter annoucments</t>
-  </si>
-  <si>
-    <t>exec delete chapter annoouncements</t>
-  </si>
-  <si>
     <t>show information based on who is logged in</t>
   </si>
   <si>
@@ -160,6 +154,15 @@
   </si>
   <si>
     <t>make responsive: http://themeloom.com/2013/02/tips-embed-google-maps-and-calendars-in-a-responsive-wordpress-theme/</t>
+  </si>
+  <si>
+    <t>add chapter annoucments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delete chapter annoouncements</t>
+  </si>
+  <si>
+    <t>exec only</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,6 +279,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -630,7 +634,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -649,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1"/>
@@ -677,7 +681,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
@@ -686,14 +690,14 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
         <v>36</v>
@@ -718,8 +722,8 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>41</v>
+      <c r="G6" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -741,8 +745,8 @@
       <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" t="s">
-        <v>42</v>
+      <c r="G7" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -758,6 +762,9 @@
       <c r="F8" t="s">
         <v>27</v>
       </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
@@ -780,7 +787,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
         <v>30</v>
@@ -796,7 +803,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7">

</xml_diff>

<commit_message>
Roster displaying email addresses
</commit_message>
<xml_diff>
--- a/TodoList.xlsx
+++ b/TodoList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,11 +275,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -681,7 +681,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
@@ -690,16 +690,16 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -722,7 +722,7 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -745,7 +745,7 @@
       <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -762,7 +762,7 @@
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -773,7 +773,7 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -781,7 +781,7 @@
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -789,7 +789,7 @@
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -802,7 +802,7 @@
       <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -812,7 +812,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>